<commit_message>
ui revisados por uds
</commit_message>
<xml_diff>
--- a/IIProyectoDiseno/build/web/WEB-INF/classes/files/DatosProyecto1.xlsx
+++ b/IIProyectoDiseno/build/web/WEB-INF/classes/files/DatosProyecto1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="PROFESORES" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="68">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -94,6 +94,9 @@
     <t xml:space="preserve">erew</t>
   </si>
   <si>
+    <t xml:space="preserve">ASISTENTE</t>
+  </si>
+  <si>
     <t xml:space="preserve">4-4444-4444</t>
   </si>
   <si>
@@ -224,99 +227,6 @@
   </si>
   <si>
     <t xml:space="preserve">B3-07</t>
-  </si>
-  <si>
-    <t>1-1111-1111</t>
-  </si>
-  <si>
-    <t>Ericka Solano Fernández</t>
-  </si>
-  <si>
-    <t>ersolano@itcr.ac.cr</t>
-  </si>
-  <si>
-    <t>8111-1111</t>
-  </si>
-  <si>
-    <t>masm</t>
-  </si>
-  <si>
-    <t>COORDINADOR</t>
-  </si>
-  <si>
-    <t>2-2222-2222</t>
-  </si>
-  <si>
-    <t>Alicia Salazar Hernández</t>
-  </si>
-  <si>
-    <t>asalazar@itcr.ac.cr</t>
-  </si>
-  <si>
-    <t>8222-2222</t>
-  </si>
-  <si>
-    <t>dfsdf</t>
-  </si>
-  <si>
-    <t>DIRECTOR</t>
-  </si>
-  <si>
-    <t>3-3333-3333</t>
-  </si>
-  <si>
-    <t>Saúl Calderón Ramírez</t>
-  </si>
-  <si>
-    <t>sacalderon@itcr.ac.cr</t>
-  </si>
-  <si>
-    <t>8333-3333</t>
-  </si>
-  <si>
-    <t>erew</t>
-  </si>
-  <si>
-    <t>4-4444-4444</t>
-  </si>
-  <si>
-    <t>Franco Quirós Ramírez</t>
-  </si>
-  <si>
-    <t>fquiros@itcr.ac.cr</t>
-  </si>
-  <si>
-    <t>8444-4444</t>
-  </si>
-  <si>
-    <t>qwkqe</t>
-  </si>
-  <si>
-    <t>5-5555-5555</t>
-  </si>
-  <si>
-    <t>Ivannia Cerdas Quesada</t>
-  </si>
-  <si>
-    <t>iquesada@itcr.ac.cr</t>
-  </si>
-  <si>
-    <t>8555-5555</t>
-  </si>
-  <si>
-    <t>qweqqqq</t>
-  </si>
-  <si>
-    <t>super</t>
-  </si>
-  <si>
-    <t>8666-6666</t>
-  </si>
-  <si>
-    <t>Disenno</t>
-  </si>
-  <si>
-    <t>SUPERUSUARIO</t>
   </si>
 </sst>
 </file>
@@ -326,7 +236,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -349,29 +259,6 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
-    <font>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FF0563C1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF0563C1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -390,7 +277,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -414,97 +301,21 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0563C1"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -516,15 +327,15 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="12.3198380566802" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="0" width="24.1012145748988" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="0" width="21.3157894736842" collapsed="true"/>
-    <col min="4" max="1025" hidden="false" style="0" width="10.6032388663968" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -547,124 +358,124 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E3" t="s">
-        <v>77</v>
-      </c>
-      <c r="F3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E4" t="s">
-        <v>83</v>
-      </c>
-      <c r="F4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D5" t="s">
-        <v>87</v>
-      </c>
-      <c r="E5" t="s">
-        <v>88</v>
-      </c>
-      <c r="F5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>89</v>
-      </c>
-      <c r="B6" t="s">
-        <v>90</v>
-      </c>
-      <c r="C6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D6" t="s">
-        <v>92</v>
-      </c>
-      <c r="E6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>94</v>
-      </c>
-      <c r="B7" t="s">
-        <v>94</v>
-      </c>
-      <c r="C7" t="s">
-        <v>94</v>
-      </c>
-      <c r="D7" t="s">
-        <v>95</v>
-      </c>
-      <c r="E7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F7" t="s">
-        <v>97</v>
+    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -699,28 +510,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="10.6032388663968" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="0" width="25.9230769230769" collapsed="true"/>
-    <col min="3" max="1025" hidden="false" style="0" width="10.6032388663968" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.515306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>3</v>
@@ -728,10 +539,10 @@
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>3</v>
@@ -739,10 +550,10 @@
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>4</v>
@@ -750,10 +561,10 @@
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>4</v>
@@ -761,10 +572,10 @@
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>4</v>
@@ -794,23 +605,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="15.2105263157895" collapsed="true"/>
-    <col min="2" max="1025" hidden="false" style="0" width="10.6032388663968" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -837,77 +648,77 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="4" hidden="false" style="0" width="10.6032388663968" collapsed="true"/>
-    <col min="5" max="5" hidden="false" style="0" width="14.6761133603239" collapsed="true"/>
-    <col min="6" max="1025" hidden="false" style="0" width="10.6032388663968" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.4438775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E3" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>61</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>1</v>
@@ -916,38 +727,38 @@
         <v>12</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E5" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" s="0" t="s">
         <v>64</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1</v>
@@ -956,18 +767,18 @@
         <v>12</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1</v>
@@ -976,18 +787,18 @@
         <v>6</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>2</v>
@@ -996,10 +807,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
creo que la progra esta!
</commit_message>
<xml_diff>
--- a/IIProyectoDiseno/build/web/WEB-INF/classes/files/DatosProyecto1.xlsx
+++ b/IIProyectoDiseno/build/web/WEB-INF/classes/files/DatosProyecto1.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="101">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -227,6 +227,105 @@
   </si>
   <si>
     <t xml:space="preserve">B3-07</t>
+  </si>
+  <si>
+    <t>1-1111-1111</t>
+  </si>
+  <si>
+    <t>Ericka Solano Fernández</t>
+  </si>
+  <si>
+    <t>ersolano@itcr.ac.cr</t>
+  </si>
+  <si>
+    <t>8111-1111</t>
+  </si>
+  <si>
+    <t>masm</t>
+  </si>
+  <si>
+    <t>COORDINADOR</t>
+  </si>
+  <si>
+    <t>2-2222-2222</t>
+  </si>
+  <si>
+    <t>Alicia Salazar Hernández</t>
+  </si>
+  <si>
+    <t>asalazar@itcr.ac.cr</t>
+  </si>
+  <si>
+    <t>8222-2222</t>
+  </si>
+  <si>
+    <t>dfsdf</t>
+  </si>
+  <si>
+    <t>DIRECTOR</t>
+  </si>
+  <si>
+    <t>4-4444-4444</t>
+  </si>
+  <si>
+    <t>Franco Quirós Ramírez</t>
+  </si>
+  <si>
+    <t>fquiros@itcr.ac.cr</t>
+  </si>
+  <si>
+    <t>8444-4444</t>
+  </si>
+  <si>
+    <t>qwkqe</t>
+  </si>
+  <si>
+    <t>5-5555-5555</t>
+  </si>
+  <si>
+    <t>Ivannia Cerdas Quesada</t>
+  </si>
+  <si>
+    <t>iquesada@itcr.ac.cr</t>
+  </si>
+  <si>
+    <t>8555-5555</t>
+  </si>
+  <si>
+    <t>qweqqqq</t>
+  </si>
+  <si>
+    <t>super</t>
+  </si>
+  <si>
+    <t>8666-6666</t>
+  </si>
+  <si>
+    <t>Disenno</t>
+  </si>
+  <si>
+    <t>SUPERUSUARIO</t>
+  </si>
+  <si>
+    <t>1-1670-0598</t>
+  </si>
+  <si>
+    <t>Ariana B</t>
+  </si>
+  <si>
+    <t>b@h.com</t>
+  </si>
+  <si>
+    <t>22609987</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>2-2222-1111</t>
+  </si>
+  <si>
+    <t>Ericka Solano Fernánde</t>
   </si>
 </sst>
 </file>
@@ -431,10 +530,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.4251012145749"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3157894736842"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.6032388663968"/>
+    <col min="1" max="1" hidden="false" style="0" width="12.4251012145749" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="24.3157894736842" collapsed="true"/>
+    <col min="3" max="3" hidden="false" style="0" width="21.5303643724696" collapsed="true"/>
+    <col min="4" max="1025" hidden="false" style="0" width="10.6032388663968" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -457,124 +556,144 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>37</v>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -609,9 +728,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0283400809717"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.6032388663968"/>
+    <col min="1" max="1" hidden="false" style="0" width="10.6032388663968" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="26.0283400809717" collapsed="true"/>
+    <col min="3" max="1025" hidden="false" style="0" width="10.6032388663968" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -704,8 +823,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.6032388663968"/>
+    <col min="1" max="1" hidden="false" style="0" width="15.3198380566802" collapsed="true"/>
+    <col min="2" max="1025" hidden="false" style="0" width="10.6032388663968" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -747,9 +866,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.7813765182186"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.6032388663968"/>
+    <col min="1" max="4" hidden="false" style="0" width="10.6032388663968" collapsed="true"/>
+    <col min="5" max="5" hidden="false" style="0" width="14.7813765182186" collapsed="true"/>
+    <col min="6" max="1025" hidden="false" style="0" width="10.6032388663968" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>